<commit_message>
Sprint review protocols added
</commit_message>
<xml_diff>
--- a/Org/Semester 2/DAGoPERT_2016_slim.xlsx
+++ b/Org/Semester 2/DAGoPERT_2016_slim.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\OneDrive\Studium\FHTechnikum\3. Semester\9_InnoLab\2_InnoLab2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\OneDrive\Studium\FHTechnikum\3. Semester\9_InnoLab\LocalRep\Org\Semester 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -676,7 +676,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -698,6 +698,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1197,7 +1203,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="192">
+  <cellXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1710,6 +1716,12 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Normal 2" xfId="2"/>
@@ -1969,11 +1981,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1675875584"/>
-        <c:axId val="-1675875040"/>
+        <c:axId val="-384578784"/>
+        <c:axId val="-384578240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1675875584"/>
+        <c:axId val="-384578784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2047,12 +2059,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1675875040"/>
+        <c:crossAx val="-384578240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1675875040"/>
+        <c:axId val="-384578240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2138,7 +2150,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1675875584"/>
+        <c:crossAx val="-384578784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2218,7 +2230,7 @@
         <xdr:cNvPr id="9218" name="Text 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002240000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002240000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2561,7 +2573,7 @@
         <xdr:cNvPr id="6162" name="Chart 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000012180000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000012180000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3203,8 +3215,8 @@
   </sheetPr>
   <dimension ref="A1:Q359"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3647,13 +3659,13 @@
       <c r="A9" s="178" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="152" t="s">
+      <c r="B9" s="192" t="s">
         <v>107</v>
       </c>
-      <c r="C9" s="152" t="s">
+      <c r="C9" s="192" t="s">
         <v>106</v>
       </c>
-      <c r="D9" s="153" t="s">
+      <c r="D9" s="193" t="s">
         <v>111</v>
       </c>
       <c r="E9" s="154">
@@ -3705,13 +3717,13 @@
       <c r="A10" s="178" t="s">
         <v>129</v>
       </c>
-      <c r="B10" s="152" t="s">
+      <c r="B10" s="192" t="s">
         <v>107</v>
       </c>
-      <c r="C10" s="152" t="s">
+      <c r="C10" s="192" t="s">
         <v>108</v>
       </c>
-      <c r="D10" s="152" t="s">
+      <c r="D10" s="192" t="s">
         <v>112</v>
       </c>
       <c r="E10" s="154">
@@ -3941,13 +3953,13 @@
       <c r="A14" s="178" t="s">
         <v>133</v>
       </c>
-      <c r="B14" s="152" t="s">
+      <c r="B14" s="192" t="s">
         <v>117</v>
       </c>
-      <c r="C14" s="152" t="s">
+      <c r="C14" s="192" t="s">
         <v>115</v>
       </c>
-      <c r="D14" s="152" t="s">
+      <c r="D14" s="192" t="s">
         <v>116</v>
       </c>
       <c r="E14" s="154">
@@ -3999,13 +4011,13 @@
       <c r="A15" s="178" t="s">
         <v>134</v>
       </c>
-      <c r="B15" s="152" t="s">
+      <c r="B15" s="192" t="s">
         <v>117</v>
       </c>
-      <c r="C15" s="152" t="s">
+      <c r="C15" s="192" t="s">
         <v>122</v>
       </c>
-      <c r="D15" s="152" t="s">
+      <c r="D15" s="192" t="s">
         <v>119</v>
       </c>
       <c r="E15" s="154">
@@ -4057,13 +4069,13 @@
       <c r="A16" s="178" t="s">
         <v>135</v>
       </c>
-      <c r="B16" s="152" t="s">
+      <c r="B16" s="192" t="s">
         <v>117</v>
       </c>
-      <c r="C16" s="152" t="s">
+      <c r="C16" s="192" t="s">
         <v>123</v>
       </c>
-      <c r="D16" s="152" t="s">
+      <c r="D16" s="192" t="s">
         <v>118</v>
       </c>
       <c r="E16" s="154">
@@ -19271,18 +19283,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19464,6 +19476,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F155915-390F-4DB1-8323-6D9C71B4FD2C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90C8B9A1-CF49-4753-98D3-CDFF9713AD0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -19474,14 +19494,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F155915-390F-4DB1-8323-6D9C71B4FD2C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>